<commit_message>
Halfway through making drawers
seriously why did we make so many categories

i should automate this but i'm lazy~
</commit_message>
<xml_diff>
--- a/categoryList.xlsx
+++ b/categoryList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SLA\Documents\Unity\github\lost-and-filed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F40F292-65B9-41FC-9BFC-C30919FFE394}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{143518DD-D4B2-403E-BE6B-33D5C5D442F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D0597EE1-D535-4591-A878-CB218FC0E56E}"/>
+    <workbookView xWindow="28680" yWindow="7095" windowWidth="24240" windowHeight="13740" xr2:uid="{D0597EE1-D535-4591-A878-CB218FC0E56E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="81">
-  <si>
-    <t>Wriswatch</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="84">
   <si>
     <t>Remote control</t>
   </si>
@@ -237,9 +234,6 @@
     <t>Child</t>
   </si>
   <si>
-    <t>Cursed video tape</t>
-  </si>
-  <si>
     <t>Dog</t>
   </si>
   <si>
@@ -277,6 +271,21 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>Interactable</t>
+  </si>
+  <si>
+    <t>Wristwatch</t>
+  </si>
+  <si>
+    <t>Done?</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Video tape</t>
   </si>
 </sst>
 </file>
@@ -637,426 +646,601 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF1BD883-602F-4198-AF5C-58AAFA80A26A}">
-  <dimension ref="A1:D76"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
         <v>50</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>51</v>
       </c>
-      <c r="D1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="E6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="D11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="D12" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="E13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="E14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="E15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="D16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="E17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="E18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="C19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C20" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="E20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="E21" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="D22" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="E23" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="D24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="C25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" t="s">
+        <v>79</v>
+      </c>
+      <c r="E25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C26" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="E26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="E27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="E28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="C29" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" t="s">
+        <v>79</v>
+      </c>
+      <c r="E29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C30" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="D30" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="E31" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="E32" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="E33" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="D34" t="s">
+        <v>79</v>
+      </c>
+      <c r="E34" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="D35" t="s">
+        <v>79</v>
+      </c>
+      <c r="E35" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="E36" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="D37" t="s">
+        <v>79</v>
+      </c>
+      <c r="E37" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="E38" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="E39" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="E40" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="D41" t="s">
+        <v>53</v>
+      </c>
+      <c r="E41" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D42" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="E42" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="E43" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="C44" t="s">
+        <v>52</v>
+      </c>
+      <c r="D44" t="s">
+        <v>79</v>
+      </c>
+      <c r="E44" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C45" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="E45" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="E46" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1064,7 +1248,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1072,7 +1256,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>31</v>
+        <v>61</v>
+      </c>
+      <c r="D50" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1080,10 +1267,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D51" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1091,7 +1278,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>60</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1099,7 +1286,13 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>1</v>
+        <v>56</v>
+      </c>
+      <c r="C53" t="s">
+        <v>52</v>
+      </c>
+      <c r="D53" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1107,10 +1300,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C54" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+      <c r="D54" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1118,7 +1311,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>56</v>
+        <v>24</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1126,7 +1319,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1134,7 +1327,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1142,7 +1335,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1150,7 +1343,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>30</v>
+        <v>57</v>
+      </c>
+      <c r="D59" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1160,16 +1356,19 @@
       <c r="B60" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="C60" t="s">
+        <v>52</v>
+      </c>
+      <c r="D60" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C61" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1177,7 +1376,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1185,7 +1384,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1193,108 +1392,120 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="D68" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="C71" t="s">
+        <v>52</v>
+      </c>
+      <c r="D71" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="D73" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>0</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:C76">
-    <sortCondition ref="B76"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:E76">
+    <sortCondition ref="B2:B76"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Game loop finished (finally)
No audio at all
</commit_message>
<xml_diff>
--- a/categoryList.xlsx
+++ b/categoryList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SLA\Documents\Unity\github\lost-and-filed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12BB116-948E-46FF-923D-A2138418DD5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650BC60C-C86B-4881-AC38-98C5ECABBF32}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="7095" windowWidth="24240" windowHeight="13740" xr2:uid="{D0597EE1-D535-4591-A878-CB218FC0E56E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="84">
   <si>
     <t>Remote control</t>
   </si>
@@ -219,9 +219,6 @@
     <t>Passport</t>
   </si>
   <si>
-    <t>Plot”</t>
-  </si>
-  <si>
     <t>Umbrella</t>
   </si>
   <si>
@@ -286,6 +283,9 @@
   </si>
   <si>
     <t>Video tape</t>
+  </si>
+  <si>
+    <t>"Plot”</t>
   </si>
 </sst>
 </file>
@@ -648,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF1BD883-602F-4198-AF5C-58AAFA80A26A}">
   <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,7 +660,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B1" t="s">
         <v>49</v>
@@ -672,7 +672,7 @@
         <v>51</v>
       </c>
       <c r="E1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -683,7 +683,7 @@
         <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -694,7 +694,7 @@
         <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -705,7 +705,7 @@
         <v>38</v>
       </c>
       <c r="E4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -716,7 +716,7 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -727,7 +727,7 @@
         <v>44</v>
       </c>
       <c r="E6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -738,7 +738,7 @@
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -749,7 +749,7 @@
         <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -760,7 +760,7 @@
         <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -771,7 +771,7 @@
         <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -779,16 +779,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
         <v>52</v>
       </c>
       <c r="D11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -796,13 +796,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -813,7 +813,7 @@
         <v>37</v>
       </c>
       <c r="E13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -824,7 +824,7 @@
         <v>43</v>
       </c>
       <c r="E14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -835,7 +835,7 @@
         <v>19</v>
       </c>
       <c r="E15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -843,13 +843,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -860,7 +860,7 @@
         <v>28</v>
       </c>
       <c r="E17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -871,7 +871,7 @@
         <v>36</v>
       </c>
       <c r="E18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -879,16 +879,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C19" t="s">
         <v>52</v>
       </c>
       <c r="D19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -896,10 +896,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -910,7 +910,7 @@
         <v>40</v>
       </c>
       <c r="E21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -918,13 +918,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -935,7 +935,7 @@
         <v>42</v>
       </c>
       <c r="E23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -943,13 +943,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -957,16 +957,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C25" t="s">
         <v>52</v>
       </c>
       <c r="D25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -977,7 +977,7 @@
         <v>23</v>
       </c>
       <c r="E26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -988,7 +988,7 @@
         <v>11</v>
       </c>
       <c r="E27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -999,7 +999,7 @@
         <v>8</v>
       </c>
       <c r="E28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1007,16 +1007,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C29" t="s">
         <v>52</v>
       </c>
       <c r="D29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E29" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1024,13 +1024,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1041,7 +1041,7 @@
         <v>16</v>
       </c>
       <c r="E31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1049,10 +1049,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1063,7 +1063,7 @@
         <v>20</v>
       </c>
       <c r="E33" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1071,13 +1071,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1085,13 +1085,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E35" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1102,7 +1102,7 @@
         <v>33</v>
       </c>
       <c r="E36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1110,13 +1110,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E37" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1127,7 +1127,7 @@
         <v>12</v>
       </c>
       <c r="E38" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1138,7 +1138,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1149,7 +1149,7 @@
         <v>2</v>
       </c>
       <c r="E40" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1163,7 +1163,7 @@
         <v>53</v>
       </c>
       <c r="E41" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1174,7 +1174,7 @@
         <v>17</v>
       </c>
       <c r="E42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1185,7 +1185,7 @@
         <v>48</v>
       </c>
       <c r="E43" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1199,10 +1199,10 @@
         <v>52</v>
       </c>
       <c r="D44" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E44" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1213,7 +1213,7 @@
         <v>31</v>
       </c>
       <c r="E45" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1224,7 +1224,7 @@
         <v>3</v>
       </c>
       <c r="E46" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1235,7 +1235,7 @@
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1246,7 +1246,7 @@
         <v>41</v>
       </c>
       <c r="E48" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1257,7 +1257,7 @@
         <v>30</v>
       </c>
       <c r="E49" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1265,13 +1265,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="D50" t="s">
         <v>53</v>
       </c>
       <c r="E50" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1282,10 +1282,10 @@
         <v>59</v>
       </c>
       <c r="D51" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E51" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1296,7 +1296,7 @@
         <v>0</v>
       </c>
       <c r="E52" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1310,10 +1310,10 @@
         <v>52</v>
       </c>
       <c r="D53" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E53" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1324,10 +1324,10 @@
         <v>55</v>
       </c>
       <c r="D54" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E54" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1338,7 +1338,7 @@
         <v>24</v>
       </c>
       <c r="E55" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -1349,7 +1349,7 @@
         <v>9</v>
       </c>
       <c r="E56" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -1360,7 +1360,7 @@
         <v>21</v>
       </c>
       <c r="E57" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -1371,7 +1371,7 @@
         <v>29</v>
       </c>
       <c r="E58" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -1382,10 +1382,10 @@
         <v>57</v>
       </c>
       <c r="D59" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E59" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -1399,10 +1399,10 @@
         <v>52</v>
       </c>
       <c r="D60" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E60" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -1413,7 +1413,7 @@
         <v>22</v>
       </c>
       <c r="E61" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -1424,7 +1424,7 @@
         <v>15</v>
       </c>
       <c r="E62" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -1435,7 +1435,7 @@
         <v>39</v>
       </c>
       <c r="E63" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -1446,7 +1446,7 @@
         <v>35</v>
       </c>
       <c r="E64" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -1457,7 +1457,7 @@
         <v>46</v>
       </c>
       <c r="E65" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -1468,7 +1468,7 @@
         <v>26</v>
       </c>
       <c r="E66" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -1479,7 +1479,7 @@
         <v>45</v>
       </c>
       <c r="E67" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -1487,13 +1487,13 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D68" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E68" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -1504,7 +1504,7 @@
         <v>47</v>
       </c>
       <c r="E69" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -1515,7 +1515,7 @@
         <v>32</v>
       </c>
       <c r="E70" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -1523,16 +1523,16 @@
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C71" t="s">
         <v>52</v>
       </c>
       <c r="D71" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E71" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -1542,16 +1542,22 @@
       <c r="B72" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="E72" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D73" t="s">
-        <v>79</v>
+        <v>78</v>
+      </c>
+      <c r="E73" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -1561,6 +1567,9 @@
       <c r="B74" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="E74" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
@@ -1569,13 +1578,19 @@
       <c r="B75" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="E75" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+      <c r="E76" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>